<commit_message>
add sch hybris oct
</commit_message>
<xml_diff>
--- a/data/расписание.xlsx
+++ b/data/расписание.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrris\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA181AE-AEFB-4E87-9AD3-57C8F476C88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C66F941-15B4-48E4-938F-C507647CB41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="495" windowWidth="29040" windowHeight="15720" tabRatio="357" activeTab="3" xr2:uid="{175AAC6D-70E5-4356-ADA7-BD37772576FC}"/>
+    <workbookView xWindow="-28920" yWindow="495" windowWidth="29040" windowHeight="15720" tabRatio="357" xr2:uid="{175AAC6D-70E5-4356-ADA7-BD37772576FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hybris" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="135">
   <si>
     <t>Комлев Владислав</t>
   </si>
@@ -420,6 +420,30 @@
   </si>
   <si>
     <t>Полунин Вадим, Демин Владимир</t>
+  </si>
+  <si>
+    <t>01.09 9:00 - 08.09 9:00</t>
+  </si>
+  <si>
+    <t>Чупринский Михаил</t>
+  </si>
+  <si>
+    <t>Парфенов Глеб, Кузовлева Светлана</t>
+  </si>
+  <si>
+    <t>08.09 9:00 - 15.09 9:00</t>
+  </si>
+  <si>
+    <t>15.09 9:00 - 22.09 9:00</t>
+  </si>
+  <si>
+    <t>22.09 9:00 - 29.09 9:00</t>
+  </si>
+  <si>
+    <t>29.09 9:00 - 06.10 9:00</t>
+  </si>
+  <si>
+    <t>06.10 9:00 - 13.10 9:00</t>
   </si>
 </sst>
 </file>
@@ -878,14 +902,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E189872A-DE30-4CF8-AAD7-6E4E006B89B5}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -924,22 +948,70 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="7"/>
@@ -955,6 +1027,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -962,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03F807C-6ACF-4A12-A9D3-ED5B0F195914}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
@@ -2055,7 +2128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E517F2-1B90-467E-A143-F03ACB3900D7}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
@@ -2994,7 +3067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8842FC67-D965-4647-AE49-E30964D40D58}">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P69" sqref="P69"/>
     </sheetView>
   </sheetViews>

</xml_diff>